<commit_message>
update songs 398 with url huiyin
</commit_message>
<xml_diff>
--- a/tools/input.xlsx
+++ b/tools/input.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="846">
   <si>
     <t>歌名</t>
   </si>
@@ -1846,6 +1846,9 @@
   </si>
   <si>
     <t>余又</t>
+  </si>
+  <si>
+    <t>https://www.bilibili.com/video/BV16UQBYLE4z</t>
   </si>
   <si>
     <t>送你一朵小红花</t>
@@ -2575,6 +2578,9 @@
   </si>
   <si>
     <t>试歌</t>
+  </si>
+  <si>
+    <t>云深不知处</t>
   </si>
   <si>
     <t>梦回花事了</t>
@@ -8038,13 +8044,16 @@
       <c r="D356" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="E356" s="8" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B357" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C357" s="0" t="s">
         <v>7</v>
@@ -8055,10 +8064,10 @@
     </row>
     <row r="358">
       <c r="A358" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B358" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C358" s="0" t="s">
         <v>7</v>
@@ -8069,10 +8078,10 @@
     </row>
     <row r="359">
       <c r="A359" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B359" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C359" s="0" t="s">
         <v>7</v>
@@ -8083,10 +8092,10 @@
     </row>
     <row r="360">
       <c r="A360" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B360" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C360" s="0" t="s">
         <v>7</v>
@@ -8097,10 +8106,10 @@
     </row>
     <row r="361">
       <c r="A361" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B361" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C361" s="0" t="s">
         <v>7</v>
@@ -8111,10 +8120,10 @@
     </row>
     <row r="362">
       <c r="A362" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B362" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C362" s="0" t="s">
         <v>7</v>
@@ -8125,10 +8134,10 @@
     </row>
     <row r="363">
       <c r="A363" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B363" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C363" s="0" t="s">
         <v>7</v>
@@ -8139,10 +8148,10 @@
     </row>
     <row r="364">
       <c r="A364" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C364" s="0" t="s">
         <v>7</v>
@@ -8153,7 +8162,7 @@
     </row>
     <row r="365">
       <c r="A365" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B365" s="0" t="s">
         <v>594</v>
@@ -8167,10 +8176,10 @@
     </row>
     <row r="366">
       <c r="A366" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C366" s="0" t="s">
         <v>7</v>
@@ -8181,10 +8190,10 @@
     </row>
     <row r="367">
       <c r="A367" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C367" s="0" t="s">
         <v>7</v>
@@ -8195,10 +8204,10 @@
     </row>
     <row r="368">
       <c r="A368" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B368" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C368" s="0" t="s">
         <v>7</v>
@@ -8209,7 +8218,7 @@
     </row>
     <row r="369">
       <c r="A369" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B369" s="0" t="s">
         <v>430</v>
@@ -8223,10 +8232,10 @@
     </row>
     <row r="370">
       <c r="A370" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B370" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C370" s="0" t="s">
         <v>7</v>
@@ -8238,10 +8247,10 @@
     </row>
     <row r="371">
       <c r="A371" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="B371" s="0" t="s">
         <v>633</v>
-      </c>
-      <c r="B371" s="0" t="s">
-        <v>632</v>
       </c>
       <c r="C371" s="0" t="s">
         <v>7</v>
@@ -8253,10 +8262,10 @@
     </row>
     <row r="372">
       <c r="A372" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C372" s="0" t="s">
         <v>7</v>
@@ -8268,10 +8277,10 @@
     </row>
     <row r="373">
       <c r="A373" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C373" s="0" t="s">
         <v>7</v>
@@ -8282,10 +8291,10 @@
     </row>
     <row r="374">
       <c r="A374" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C374" s="0" t="s">
         <v>7</v>
@@ -8296,10 +8305,10 @@
     </row>
     <row r="375">
       <c r="A375" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C375" s="0" t="s">
         <v>7</v>
@@ -8310,10 +8319,10 @@
     </row>
     <row r="376">
       <c r="A376" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C376" s="0" t="s">
         <v>7</v>
@@ -8324,7 +8333,7 @@
     </row>
     <row r="377">
       <c r="A377" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B377" s="0" t="s">
         <v>387</v>
@@ -8338,7 +8347,7 @@
     </row>
     <row r="378">
       <c r="A378" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B378" s="0" t="s">
         <v>387</v>
@@ -8352,7 +8361,7 @@
     </row>
     <row r="379">
       <c r="A379" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B379" s="0" t="s">
         <v>387</v>
@@ -8380,7 +8389,7 @@
     </row>
     <row r="381">
       <c r="A381" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B381" s="0" t="s">
         <v>387</v>
@@ -8394,7 +8403,7 @@
     </row>
     <row r="382">
       <c r="A382" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B382" s="0" t="s">
         <v>387</v>
@@ -8408,7 +8417,7 @@
     </row>
     <row r="383">
       <c r="A383" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B383" s="0" t="s">
         <v>387</v>
@@ -8422,7 +8431,7 @@
     </row>
     <row r="384">
       <c r="A384" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B384" s="0" t="s">
         <v>387</v>
@@ -8436,7 +8445,7 @@
     </row>
     <row r="385">
       <c r="A385" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B385" s="0" t="s">
         <v>387</v>
@@ -8450,7 +8459,7 @@
     </row>
     <row r="386">
       <c r="A386" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B386" s="0" t="s">
         <v>387</v>
@@ -8464,7 +8473,7 @@
     </row>
     <row r="387">
       <c r="A387" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B387" s="0" t="s">
         <v>387</v>
@@ -8478,10 +8487,10 @@
     </row>
     <row r="388">
       <c r="A388" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B388" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C388" s="0" t="s">
         <v>7</v>
@@ -8492,7 +8501,7 @@
     </row>
     <row r="389">
       <c r="A389" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B389" s="0" t="s">
         <v>546</v>
@@ -8506,7 +8515,7 @@
     </row>
     <row r="390">
       <c r="A390" s="3" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B390" s="0" t="s">
         <v>546</v>
@@ -8520,7 +8529,7 @@
     </row>
     <row r="391">
       <c r="A391" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B391" s="0" t="s">
         <v>430</v>
@@ -8534,10 +8543,10 @@
     </row>
     <row r="392">
       <c r="A392" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B392" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C392" s="0" t="s">
         <v>7</v>
@@ -8548,7 +8557,7 @@
     </row>
     <row r="393">
       <c r="A393" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B393" s="0" t="s">
         <v>55</v>
@@ -8562,10 +8571,10 @@
     </row>
     <row r="394">
       <c r="A394" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B394" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C394" s="0" t="s">
         <v>7</v>
@@ -8576,10 +8585,10 @@
     </row>
     <row r="395">
       <c r="A395" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B395" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C395" s="0" t="s">
         <v>7</v>
@@ -8590,7 +8599,7 @@
     </row>
     <row r="396">
       <c r="A396" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B396" s="0" t="s">
         <v>236</v>
@@ -8604,10 +8613,10 @@
     </row>
     <row r="397">
       <c r="A397" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C397" s="0" t="s">
         <v>7</v>
@@ -8618,7 +8627,7 @@
     </row>
     <row r="398">
       <c r="A398" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B398" s="0" t="s">
         <v>55</v>
@@ -8632,10 +8641,10 @@
     </row>
     <row r="399">
       <c r="A399" s="3" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B399" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C399" s="0" t="s">
         <v>7</v>
@@ -8674,6 +8683,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E302" display="https://www.bilibili.com/video/BV12WY5ebEDC" r:id="rId26"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E161" display="https://www.bilibili.com/video/BV1fobXe1EW1" r:id="rId27"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E214" display="https://www.bilibili.com/video/BV1NFqKYZEx9" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E356" display="https://www.bilibili.com/video/BV16UQBYLE4z" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8701,266 +8711,266 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="4" ht="60" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="5" ht="60" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="6" ht="60" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="7" ht="60" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="13" ht="60" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="14" ht="60" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="15" ht="60" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="16" ht="60" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="17" ht="60" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="18" ht="60" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="19" ht="60" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="20" ht="60" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="21" ht="60" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="22" ht="60" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="23" ht="60" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="24" ht="60" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="25" ht="60" customHeight="1"/>
@@ -8999,423 +9009,423 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E1" s="0" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -9470,39 +9480,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>665</v>
+        <v>844</v>
       </c>
       <c r="B5" s="0" t="n"/>
       <c r="C5" s="0" t="n"/>
       <c r="D5" s="0" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>667</v>
-      </c>
+      <c r="A6" s="0" t="n"/>
       <c r="B6" s="0" t="n"/>
       <c r="C6" s="0" t="n"/>
       <c r="D6" s="0" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>668</v>
-      </c>
+      <c r="A7" s="3" t="n"/>
       <c r="B7" s="0" t="n"/>
       <c r="C7" s="0" t="n"/>
       <c r="D7" s="0" t="n"/>
@@ -9515,7 +9521,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
     </row>
     <row r="11">

</xml_diff>